<commit_message>
Fixed minor bugs in CIM
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/Test_IPA_5_bus_feeder.xlsx
+++ b/Grids_and_profiles/grids/Test_IPA_5_bus_feeder.xlsx
@@ -39,7 +39,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Grid</t>
+    <t>Test_IPA_5_bus_feeder</t>
   </si>
   <si>
     <t>Comments</t>
@@ -93,7 +93,7 @@
     <t>True</t>
   </si>
   <si>
-    <t>10</t>
+    <t>10.0</t>
   </si>
   <si>
     <t>0.9</t>
@@ -102,13 +102,13 @@
     <t>1.1</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>-241.9002982070312</t>
-  </si>
-  <si>
-    <t>-198.60019880468744</t>
+    <t>0j</t>
+  </si>
+  <si>
+    <t>-547.002522352756</t>
+  </si>
+  <si>
+    <t>-435.2842729412822</t>
   </si>
   <si>
     <t>20.0</t>
@@ -129,37 +129,40 @@
     <t>False</t>
   </si>
   <si>
-    <t>-124.0</t>
-  </si>
-  <si>
-    <t>27.0</t>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>-490.0</t>
+  </si>
+  <si>
+    <t>-176.0</t>
   </si>
   <si>
     <t>Bus 3</t>
   </si>
   <si>
-    <t>39.90029820703123</t>
-  </si>
-  <si>
-    <t>337.82252481953105</t>
+    <t>-327.0</t>
+  </si>
+  <si>
+    <t>134.0</t>
   </si>
   <si>
     <t>Bus 4</t>
   </si>
   <si>
-    <t>295.2622067320311</t>
-  </si>
-  <si>
-    <t>744.8055665312495</t>
+    <t>-71.0</t>
+  </si>
+  <si>
+    <t>541.0</t>
   </si>
   <si>
     <t>Bus 5</t>
   </si>
   <si>
-    <t>590.5244134640621</t>
-  </si>
-  <si>
-    <t>1117.2083497968742</t>
+    <t>224.0</t>
+  </si>
+  <si>
+    <t>914.0</t>
   </si>
   <si>
     <t>bus_from</t>
@@ -210,7 +213,7 @@
     <t>0.05</t>
   </si>
   <si>
-    <t>1e-20</t>
+    <t>1.0000000000000001e-20</t>
   </si>
   <si>
     <t>1.0</t>
@@ -231,7 +234,7 @@
     <t>4.5</t>
   </si>
   <si>
-    <t>0.056</t>
+    <t>0.055999999999999994</t>
   </si>
   <si>
     <t>0.5</t>
@@ -259,9 +262,6 @@
   </si>
   <si>
     <t>Load@Bus 5</t>
-  </si>
-  <si>
-    <t>0j</t>
   </si>
   <si>
     <t>(2+3j)</t>
@@ -843,7 +843,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -855,10 +855,10 @@
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
         <v>29</v>
@@ -881,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -890,7 +890,7 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -902,10 +902,10 @@
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -928,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -937,7 +937,7 @@
         <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
@@ -949,10 +949,10 @@
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
         <v>29</v>
@@ -975,7 +975,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -984,7 +984,7 @@
         <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -996,10 +996,10 @@
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
         <v>29</v>
@@ -1041,43 +1041,43 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -1097,34 +1097,34 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
         <v>61</v>
       </c>
-      <c r="K2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
       <c r="O2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1132,46 +1132,46 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="O3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1179,46 +1179,46 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
       </c>
       <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s">
         <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1226,46 +1226,46 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="O5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1292,25 +1292,25 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1318,19 +1318,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
         <v>80</v>
@@ -1366,19 +1366,19 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1405,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1441,10 +1441,10 @@
         <v>90</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>91</v>
@@ -1486,7 +1486,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1519,10 +1519,10 @@
         <v>90</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1549,7 +1549,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1558,10 +1558,10 @@
         <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>